<commit_message>
Working, need to initiate an update or delete to get to input boxes
</commit_message>
<xml_diff>
--- a/budget.xlsx
+++ b/budget.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>200</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5">
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>100</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6">
@@ -481,6 +481,16 @@
       </c>
       <c r="B6" t="n">
         <v>259.62</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>savings</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chart and buttons seem to work
</commit_message>
<xml_diff>
--- a/budget.xlsx
+++ b/budget.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,6 +473,16 @@
         <v>200</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>remaining</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>542.15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>